<commit_message>
adding "clean_map" to tma1 and tma2
</commit_message>
<xml_diff>
--- a/inst/extdata/tma1/example_er.xlsx
+++ b/inst/extdata/tma1/example_er.xlsx
@@ -1,22 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/tma1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4FC4166-0730-6143-90A6-2333F0D3494E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
     <sheet name="ER" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,13 +79,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -97,7 +131,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -131,6 +165,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -165,9 +200,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -340,14 +376,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>1</v>
       </c>
@@ -373,7 +411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>5</v>
       </c>
@@ -399,7 +437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>9</v>
       </c>
@@ -425,7 +463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>11</v>
       </c>
@@ -457,179 +495,115 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2">
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing up tma1 example to be more realistic
</commit_message>
<xml_diff>
--- a/inst/extdata/tma1/example_er.xlsx
+++ b/inst/extdata/tma1/example_er.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/tma1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4FC4166-0730-6143-90A6-2333F0D3494E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C9222-5AAB-3040-B18F-923235B9BB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="18380" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="1">
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -71,8 +59,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,15 +366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:L8"/>
+  <dimension ref="C2:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>1</v>
       </c>
@@ -393,42 +382,51 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
       <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>7</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="J2">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
       <c r="F3">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K3">
         <v>8</v>
@@ -436,39 +434,71 @@
       <c r="L3">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
       </c>
       <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>15</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C8">
         <v>13</v>
       </c>
-      <c r="J7">
-        <v>13</v>
-      </c>
-      <c r="K7">
-        <v>14</v>
-      </c>
-      <c r="L7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C8">
-        <v>11</v>
-      </c>
       <c r="D8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -476,17 +506,34 @@
       <c r="F8">
         <v>12</v>
       </c>
-      <c r="I8">
-        <v>15</v>
-      </c>
-      <c r="J8">
-        <v>15</v>
+      <c r="G8">
+        <v>11</v>
       </c>
       <c r="K8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L8">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="M8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -496,113 +543,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C2:L8"/>
+  <dimension ref="C2:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Debugging error - changed metadata type to "text"
</commit_message>
<xml_diff>
--- a/inst/extdata/tma1/example_er.xlsx
+++ b/inst/extdata/tma1/example_er.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/tma1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C9222-5AAB-3040-B18F-923235B9BB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C35F9E6-FA82-E146-B322-754A37AD2012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="18380" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="440" yWindow="500" windowWidth="18380" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,7 +368,7 @@
   <dimension ref="C2:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -546,22 +545,22 @@
   <dimension ref="C2:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C2" s="1">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
@@ -570,10 +569,10 @@
       <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
         <v>2</v>
       </c>
       <c r="L2" t="s">
@@ -584,28 +583,28 @@
       </c>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
@@ -642,25 +641,25 @@
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="1">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <v>2</v>
       </c>
       <c r="L7" t="s">
@@ -671,29 +670,28 @@
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C8" s="1">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
         <v>9</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>9</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changing example tma1 file name
</commit_message>
<xml_diff>
--- a/inst/extdata/tma1/example_er.xlsx
+++ b/inst/extdata/tma1/example_er.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/tma1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C35F9E6-FA82-E146-B322-754A37AD2012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752147FB-7B62-FE4D-BB96-23672D47E725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="500" windowWidth="18380" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
-    <sheet name="ER" sheetId="2" r:id="rId2"/>
+    <sheet name="er" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -545,7 +545,7 @@
   <dimension ref="C2:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix tab names in input TMAs, reorder columns in final output, test quantitative method
</commit_message>
<xml_diff>
--- a/inst/extdata/tma1/example_er.xlsx
+++ b/inst/extdata/tma1/example_er.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahokada/Documents/TMAtools/inst/extdata/tma1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/bianca_ribeiro_ubc_ca/Documents/TMAtools/inst/extdata/tma1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752147FB-7B62-FE4D-BB96-23672D47E725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{752147FB-7B62-FE4D-BB96-23672D47E725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87ADE455-7A86-4101-AC66-A07C012B43A1}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="500" windowWidth="18380" windowHeight="11600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
-    <sheet name="er" sheetId="2" r:id="rId2"/>
+    <sheet name="ER" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -371,9 +371,9 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C2">
         <v>1</v>
       </c>
@@ -405,7 +405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>4</v>
       </c>
@@ -437,7 +437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>4</v>
       </c>
@@ -460,7 +460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>10</v>
       </c>
@@ -492,7 +492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>13</v>
       </c>
@@ -518,7 +518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>13</v>
       </c>
@@ -548,9 +548,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C2">
         <v>9</v>
       </c>
@@ -582,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>2</v>
       </c>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>0</v>
       </c>
@@ -637,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -669,7 +669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>9</v>
       </c>
@@ -695,7 +695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>1</v>
       </c>

</xml_diff>